<commit_message>
int data from van
</commit_message>
<xml_diff>
--- a/public/assets/trainings Van 1.xlsx
+++ b/public/assets/trainings Van 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanessa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\EMEAREPORT\my-app\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20D94405-CBA0-4382-93AA-6F2A217A17C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6D0F1E-B014-4275-9243-13B50B046ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1C707ED-ABBF-460A-9BE8-2196CE93EDD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E1C707ED-ABBF-460A-9BE8-2196CE93EDD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -315,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -788,22 +788,22 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -829,7 +829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -855,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -881,7 +881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -907,7 +907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -933,7 +933,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -959,7 +959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -985,7 +985,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
@@ -1451,13 +1451,13 @@
         <v>784</v>
       </c>
       <c r="G25" s="4">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>8</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>8</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>8</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>8</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>8</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>8</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="s">
         <v>8</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
         <v>8</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>8</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
         <v>8</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
         <v>8</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
         <v>8</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
         <v>8</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
         <v>8</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="s">
         <v>8</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>8</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>8</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>8</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="s">
         <v>8</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="s">
         <v>8</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
         <v>8</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="s">
         <v>8</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>8</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>63</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>63</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>63</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>63</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="13" t="s">
         <v>63</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>63</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="13" t="s">
         <v>63</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="13" t="s">
         <v>63</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
         <v>63</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>63</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="13" t="s">
         <v>63</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="13" t="s">
         <v>63</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="13" t="s">
         <v>63</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="13" t="s">
         <v>63</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="13" t="s">
         <v>63</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="13" t="s">
         <v>63</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="13" t="s">
         <v>63</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="13" t="s">
         <v>63</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="13" t="s">
         <v>63</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="13" t="s">
         <v>63</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="13" t="s">
         <v>63</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="13" t="s">
         <v>63</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
         <v>63</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="13" t="s">
         <v>63</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="18" t="s">
         <v>63</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="18" t="s">
         <v>63</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="18" t="s">
         <v>63</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="18" t="s">
         <v>63</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="18" t="s">
         <v>63</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="18" t="s">
         <v>63</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="18" t="s">
         <v>63</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="18" t="s">
         <v>63</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="18" t="s">
         <v>63</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="18" t="s">
         <v>63</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="18" t="s">
         <v>63</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
         <v>63</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="18" t="s">
         <v>63</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="18" t="s">
         <v>63</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
         <v>63</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="18" t="s">
         <v>63</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="18" t="s">
         <v>63</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="18" t="s">
         <v>63</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="18" t="s">
         <v>63</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="18" t="s">
         <v>63</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="18" t="s">
         <v>63</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="18" t="s">
         <v>63</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="18" t="s">
         <v>63</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="18" t="s">
         <v>63</v>
       </c>

</xml_diff>